<commit_message>
Test case 5 added
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>UserName</t>
   </si>
@@ -52,35 +53,92 @@
     <t>Build</t>
   </si>
   <si>
+    <t>Username or Password is invalid. Please try again.</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>actiTIME - Login</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Repassword</t>
+  </si>
+  <si>
+    <t>Working schedule</t>
+  </si>
+  <si>
+    <t>Search Name</t>
+  </si>
+  <si>
+    <t>http://localhost/login.do</t>
+  </si>
+  <si>
+    <t>shekhar</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>pakale</t>
+  </si>
+  <si>
+    <t>shekhar123</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>shekhar.pakale@gmail.com</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>actiTIME - User List</t>
+  </si>
+  <si>
+    <t>shekharp123</t>
+  </si>
+  <si>
     <t>(build 39769)</t>
-  </si>
-  <si>
-    <t>Username or Password is invalid. Please try again.</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>@</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>actiTIME - Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,13 +166,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,17 +197,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +550,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -518,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -529,45 +610,45 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -607,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,10 +717,132 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="7">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test case no 06 added
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
   <si>
     <t>UserName</t>
   </si>
@@ -513,7 +514,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -688,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -730,7 +731,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,4 +846,127 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="7">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>